<commit_message>
Body02, body03 e figuras
</commit_message>
<xml_diff>
--- a/figs/body02/FIGCABLELIST.xlsx
+++ b/figs/body02/FIGCABLELIST.xlsx
@@ -14,8 +14,9 @@
   <sheets>
     <sheet name="Cable List" sheetId="1" r:id="rId1"/>
     <sheet name="Connector List" sheetId="6" r:id="rId2"/>
-    <sheet name="Cable Order" sheetId="4" r:id="rId3"/>
-    <sheet name="Cable Order 2" sheetId="5" r:id="rId4"/>
+    <sheet name="Cable type list" sheetId="7" r:id="rId3"/>
+    <sheet name="Cable Order" sheetId="4" r:id="rId4"/>
+    <sheet name="Cable Order 2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cable List'!$A$1:$K$68</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="290">
   <si>
     <t>Origin</t>
   </si>
@@ -583,9 +584,6 @@
   </si>
   <si>
     <t>DB9F(SH) / SH-Pass</t>
-  </si>
-  <si>
-    <t>10pinF / SH-Cut</t>
   </si>
   <si>
     <t>DB9M(SH) / SH-Pass</t>
@@ -940,6 +938,12 @@
   </si>
   <si>
     <t>Cable Signal Type</t>
+  </si>
+  <si>
+    <t>Length to be purchased (mm)</t>
+  </si>
+  <si>
+    <t>10pinF(CAN) / SH-Cut</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1471,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1488,7 +1492,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="23" customFormat="1" ht="36" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>2</v>
@@ -1497,19 +1501,19 @@
         <v>0</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>176</v>
@@ -1532,19 +1536,19 @@
         <v>56</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>177</v>
@@ -1567,19 +1571,19 @@
         <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>177</v>
@@ -1602,19 +1606,19 @@
         <v>58</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>177</v>
@@ -1643,13 +1647,13 @@
         <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>177</v>
@@ -1678,13 +1682,13 @@
         <v>59</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>177</v>
@@ -1719,7 +1723,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>177</v>
@@ -1742,19 +1746,19 @@
         <v>142</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>143</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>177</v>
@@ -1777,19 +1781,19 @@
         <v>143</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>144</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>177</v>
@@ -1824,7 +1828,7 @@
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>177</v>
@@ -1853,13 +1857,13 @@
         <v>144</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>177</v>
@@ -1888,13 +1892,13 @@
         <v>142</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>177</v>
@@ -1923,13 +1927,13 @@
         <v>156</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>184</v>
+        <v>289</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>177</v>
@@ -1964,7 +1968,7 @@
         <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>177</v>
@@ -1999,7 +2003,7 @@
         <v>9</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>177</v>
@@ -2028,13 +2032,13 @@
         <v>157</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>184</v>
+        <v>289</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>177</v>
@@ -2057,19 +2061,19 @@
         <v>149</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>177</v>
@@ -2092,19 +2096,19 @@
         <v>152</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>150</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>177</v>
@@ -2127,19 +2131,19 @@
         <v>154</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>153</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>177</v>
@@ -2162,19 +2166,19 @@
         <v>155</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>160</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>177</v>
@@ -2197,25 +2201,25 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="I21" s="1" t="s">
         <v>51</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>51</v>
@@ -2232,25 +2236,25 @@
         <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="I22" s="1" t="s">
         <v>51</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>51</v>
@@ -2258,7 +2262,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>3</v>
@@ -2267,19 +2271,19 @@
         <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>51</v>
@@ -2293,7 +2297,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>3</v>
@@ -2302,19 +2306,19 @@
         <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>51</v>
@@ -2328,7 +2332,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -2337,19 +2341,19 @@
         <v>58</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>51</v>
@@ -2363,7 +2367,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>3</v>
@@ -2372,19 +2376,19 @@
         <v>59</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>51</v>
@@ -2398,7 +2402,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>7</v>
@@ -2407,19 +2411,19 @@
         <v>142</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>51</v>
@@ -2433,7 +2437,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
@@ -2442,19 +2446,19 @@
         <v>143</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>51</v>
@@ -2468,7 +2472,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
@@ -2477,19 +2481,19 @@
         <v>144</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>51</v>
@@ -2503,7 +2507,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>3</v>
@@ -2512,19 +2516,19 @@
         <v>56</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>51</v>
@@ -2538,7 +2542,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>3</v>
@@ -2547,19 +2551,19 @@
         <v>57</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>51</v>
@@ -2573,7 +2577,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>3</v>
@@ -2582,19 +2586,19 @@
         <v>58</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>51</v>
@@ -2608,7 +2612,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>3</v>
@@ -2617,19 +2621,19 @@
         <v>59</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>51</v>
@@ -2643,7 +2647,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
@@ -2652,19 +2656,19 @@
         <v>142</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>51</v>
@@ -2678,7 +2682,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
@@ -2687,19 +2691,19 @@
         <v>143</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>51</v>
@@ -2713,7 +2717,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
@@ -2722,19 +2726,19 @@
         <v>144</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>51</v>
@@ -2757,19 +2761,19 @@
         <v>56</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>51</v>
@@ -2792,19 +2796,19 @@
         <v>57</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>51</v>
@@ -2827,19 +2831,19 @@
         <v>58</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>51</v>
@@ -2862,19 +2866,19 @@
         <v>59</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>51</v>
@@ -2888,7 +2892,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
@@ -2897,19 +2901,19 @@
         <v>142</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>51</v>
@@ -2923,7 +2927,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>7</v>
@@ -2932,19 +2936,19 @@
         <v>143</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>51</v>
@@ -2958,7 +2962,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
@@ -2967,19 +2971,19 @@
         <v>144</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>51</v>
@@ -3002,22 +3006,22 @@
         <v>148</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G44" s="22" t="s">
         <v>4</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J44" s="1">
         <v>410</v>
@@ -3037,22 +3041,22 @@
         <v>149</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J45" s="1">
         <v>410</v>
@@ -3072,22 +3076,22 @@
         <v>158</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>136</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J46" s="1">
         <v>170</v>
@@ -3107,22 +3111,22 @@
         <v>151</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J47" s="1">
         <v>410</v>
@@ -3142,22 +3146,22 @@
         <v>152</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J48" s="1">
         <v>410</v>
@@ -3177,22 +3181,22 @@
         <v>158</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>136</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J49" s="1">
         <v>170</v>
@@ -3212,22 +3216,22 @@
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J50" s="1">
         <v>410</v>
@@ -3247,22 +3251,22 @@
         <v>154</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I51" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J51" s="1">
         <v>410</v>
@@ -3282,22 +3286,22 @@
         <v>158</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>136</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J52" s="1">
         <v>170</v>
@@ -3317,22 +3321,22 @@
         <v>158</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>156</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I53" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J53" s="1">
         <v>170</v>
@@ -3352,22 +3356,22 @@
         <v>153</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H54" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J54" s="1">
         <v>410</v>
@@ -3387,22 +3391,22 @@
         <v>155</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H55" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J55" s="1">
         <v>410</v>
@@ -3422,22 +3426,22 @@
         <v>158</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>159</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I56" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J56" s="1">
         <v>190</v>
@@ -3457,22 +3461,22 @@
         <v>158</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>136</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J57" s="1">
         <v>170</v>
@@ -3492,22 +3496,22 @@
         <v>158</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J58" s="1">
         <v>800</v>
@@ -3527,22 +3531,22 @@
         <v>158</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J59" s="1">
         <v>800</v>
@@ -3562,22 +3566,22 @@
         <v>158</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J60" s="1">
         <v>800</v>
@@ -3597,22 +3601,22 @@
         <v>158</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>157</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J61" s="1">
         <v>170</v>
@@ -3632,22 +3636,22 @@
         <v>149</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J62" s="1">
         <v>1000</v>
@@ -3667,22 +3671,22 @@
         <v>152</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>150</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J63" s="1">
         <v>1000</v>
@@ -3702,22 +3706,22 @@
         <v>154</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>153</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J64" s="1">
         <v>1000</v>
@@ -3737,22 +3741,22 @@
         <v>155</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>160</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I65" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J65" s="1">
         <v>1000</v>
@@ -3772,19 +3776,19 @@
         <v>12</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F66" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="G66" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="H66" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>51</v>
@@ -3807,22 +3811,22 @@
         <v>12</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J67" s="1">
         <v>350</v>
@@ -3842,22 +3846,22 @@
         <v>12</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J68" s="1">
         <v>350</v>
@@ -3900,15 +3904,15 @@
         <v>178</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>173</v>
@@ -3930,10 +3934,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="19">
         <v>2</v>
@@ -3941,10 +3945,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>186</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>187</v>
       </c>
       <c r="C5" s="19">
         <v>18</v>
@@ -3952,10 +3956,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C6" s="19">
         <v>4</v>
@@ -3963,10 +3967,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C7" s="19">
         <v>4</v>
@@ -3974,10 +3978,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C8" s="19">
         <v>40</v>
@@ -3985,10 +3989,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>206</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>207</v>
       </c>
       <c r="C9" s="19">
         <v>12</v>
@@ -3996,10 +4000,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C10" s="19">
         <v>4</v>
@@ -4007,10 +4011,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" s="19">
         <v>4</v>
@@ -4018,10 +4022,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" s="19">
         <v>4</v>
@@ -4029,10 +4033,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="19">
         <v>4</v>
@@ -4040,10 +4044,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C14" s="19">
         <v>4</v>
@@ -4051,10 +4055,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>218</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>219</v>
       </c>
       <c r="C15" s="19">
         <v>4</v>
@@ -4062,10 +4066,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C16" s="19">
         <v>4</v>
@@ -4073,10 +4077,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C17" s="19">
         <v>4</v>
@@ -4084,10 +4088,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>237</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>238</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>51</v>
@@ -4095,10 +4099,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>51</v>
@@ -4106,10 +4110,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C20" s="19">
         <v>1</v>
@@ -4117,10 +4121,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C21" s="19">
         <v>1</v>
@@ -4131,12 +4135,12 @@
         <v>179</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>175</v>
@@ -4144,7 +4148,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>174</v>
@@ -4152,7 +4156,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>180</v>
@@ -4164,6 +4168,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="23" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10890</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1050</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -4320,12 +4401,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>